<commit_message>
[#65120138] add more leds to casa.xls
</commit_message>
<xml_diff>
--- a/casa.xlsx
+++ b/casa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Single RGB led stripes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="80">
   <si>
     <t>Teto_NO:</t>
   </si>
@@ -144,9 +144,6 @@
     <t>usa SKU diferentes para leds, power/IR e conectores</t>
   </si>
   <si>
-    <t>http://dx.com/p/jr-5050-waterproof-72w-4500lm-625nm-300-led-rgb-decoration-light-strip-w-2-flat-pin-plug-5m-184665</t>
-  </si>
-  <si>
     <t>JR-5050 Waterproof 72W 4500lm 625nm 300-LED RGB Decoration Light Strip w/ EU Plug (5m)</t>
   </si>
   <si>
@@ -168,36 +165,21 @@
     <t>5050RGB 12W 200lm 60 SMD 5050 LED Waterproof RGB Light Stripe w/ 44 Key Remote Control - White (1 M)</t>
   </si>
   <si>
-    <t>http://dx.com/p/5050rgb-12w-200lm-60-smd-5050-led-waterproof-rgb-light-stripe-w-44-key-remote-control-white-1-m-263808</t>
-  </si>
-  <si>
     <t>5050RGB 12W 200lm IP65 Waterproof 60 5050 SMD LED RGB Stripe w/ Remote Control - White (110cm)</t>
   </si>
   <si>
-    <t>http://dx.com/p/5050rgb-12w-200lm-ip65-waterproof-60-5050-smd-led-rgb-stripe-w-remote-control-white-254040</t>
-  </si>
-  <si>
     <t>Single RGB led stripes</t>
   </si>
   <si>
     <t>60W 4200lm 300-5050 SMD LED RGB Flexible Decoration Stripe Lamp w/ 24-Key Controller (5m / 100~240V)</t>
   </si>
   <si>
-    <t>http://dx.com/p/60w-4200lm-300-5050-smd-led-rgb-flexible-decoration-stripe-lamp-w-24-key-controller-100-240v-265552</t>
-  </si>
-  <si>
     <t>WZJ015 10W 450lm LED RGB Project Lamp (85~265V)</t>
   </si>
   <si>
-    <t>http://dx.com/p/wzj015-10w-450lm-led-rgb-project-lamp-85-265v-264070</t>
-  </si>
-  <si>
     <t>Rate</t>
   </si>
   <si>
-    <t>Spec</t>
-  </si>
-  <si>
     <t>SKUs</t>
   </si>
   <si>
@@ -216,26 +198,71 @@
     <t>JZ-5050 Waterproof 72W 4300lm 300-SMD 5050 LED RGB Light Strip - Black + White (12V / 5m)</t>
   </si>
   <si>
-    <t>http://dx.com/p/jz-5050-waterproof-72w-4300lm-300-smd-5050-led-rgb-light-strip-black-white-228618</t>
-  </si>
-  <si>
     <t>somente led</t>
   </si>
   <si>
     <t>led, IR e power</t>
   </si>
   <si>
-    <t>http://dx.com/p/24-key-ir-remote-control-power-adapter-for-rgb-lamp-black-100-240v-264422</t>
-  </si>
-  <si>
     <t>24-key IR Remote Control + Power Adapter for RGB Lamp - Black (100~240V) 12V / 5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borui BR-QP1E27 0V RGB 10W 600LM Remoto Lâmpada LED RGB Controle Light - Prata + Branco (220V) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E27 3W 1-LED Multi-Colored Luz RGB lâmpada w / Controle Remoto (85 ~ 265V AC) </t>
+  </si>
+  <si>
+    <t>Bulbo LED4Wb-RGB E27 4W 220LM LED RGB Luz w / Função Controle Remoto / Memória (85 ~ 265V)</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>E27 5W 150LM LED RGB Luz Controle Remoto - Prata + Branco (AC 85 ~ 265V)</t>
+  </si>
+  <si>
+    <t>Mini E27 3W 90lm RGB lâmpada LED Regulável w / controle remoto (AC 85 ~ 265V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XLZM-RGB3QPD-D E27 3W 150LM 3-LED RGB Light Bulb - Prata + Branco (AC 85 ~ 265V) </t>
+  </si>
+  <si>
+    <t>10-15W Bulb</t>
+  </si>
+  <si>
+    <t>10-15W Stripe</t>
+  </si>
+  <si>
+    <t>50-100W Stripe</t>
+  </si>
+  <si>
+    <t>3-9W Bulb</t>
+  </si>
+  <si>
+    <t>($/W)</t>
+  </si>
+  <si>
+    <t>Potência</t>
+  </si>
+  <si>
+    <t>LEDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KINFIRE E27 10W sete cores RGB lâmpada LED w / controle remoto - White + Prata (85 ~ 265V) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JR-E27-7W-WW E27 7W 600lm 3300K 7-LED Branco Quente Lâmpada - Branco + Ouro + Prata </t>
+  </si>
+  <si>
+    <t>Qnt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +321,52 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +382,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,7 +470,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,20 +559,114 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -795,8 +966,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="F6" workbookViewId="0">
+      <pane ySplit="915" activePane="bottomLeft"/>
+      <selection activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,7 +985,7 @@
     <col min="12" max="12" width="95.85546875" style="5" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="30"/>
     <col min="14" max="14" width="9.140625" style="2"/>
-    <col min="15" max="15" width="9.140625" style="35"/>
+    <col min="15" max="15" width="9.140625" style="34"/>
     <col min="16" max="16" width="9.140625" style="30"/>
     <col min="17" max="17" width="9.140625" style="2"/>
   </cols>
@@ -822,15 +995,15 @@
         <v>35</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="2:18">
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:18">
@@ -845,12 +1018,12 @@
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="27" t="s">
         <v>33</v>
       </c>
@@ -862,13 +1035,13 @@
       </c>
       <c r="K6" s="29"/>
       <c r="L6" s="26" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O6" s="31" t="s">
         <v>33</v>
@@ -897,17 +1070,17 @@
       <c r="K7" s="29"/>
       <c r="L7" s="25"/>
       <c r="M7" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" s="28"/>
       <c r="O7" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P7" s="32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:18">
@@ -943,7 +1116,7 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M8" s="30">
         <v>14.3</v>
@@ -951,7 +1124,7 @@
       <c r="N8" s="2">
         <v>0</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="34">
         <f>+N8*M8</f>
         <v>0</v>
       </c>
@@ -995,7 +1168,7 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M9" s="30">
         <v>11.99</v>
@@ -1003,7 +1176,7 @@
       <c r="N9" s="2">
         <v>0</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="34">
         <f t="shared" ref="O9:O11" si="3">+N9*M9</f>
         <v>0</v>
       </c>
@@ -1047,7 +1220,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M10" s="30">
         <v>42.96</v>
@@ -1055,7 +1228,7 @@
       <c r="N10" s="2">
         <v>0</v>
       </c>
-      <c r="O10" s="35">
+      <c r="O10" s="34">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1099,7 +1272,7 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M11" s="30">
         <v>35.99</v>
@@ -1107,7 +1280,7 @@
       <c r="N11" s="2">
         <v>2</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="34">
         <f t="shared" si="3"/>
         <v>71.98</v>
       </c>
@@ -1118,7 +1291,7 @@
         <v>300</v>
       </c>
       <c r="R11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:18">
@@ -1154,15 +1327,15 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M12" s="37">
+        <v>59</v>
+      </c>
+      <c r="M12" s="36">
         <v>21.5</v>
       </c>
       <c r="N12" s="2">
         <v>0</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="34">
         <f t="shared" ref="O12" si="4">+N12*M12</f>
         <v>0</v>
       </c>
@@ -1173,7 +1346,7 @@
         <v>300</v>
       </c>
       <c r="R12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:18">
@@ -1395,7 +1568,7 @@
         <f>SUM(N8:N18)</f>
         <v>2</v>
       </c>
-      <c r="O19" s="36">
+      <c r="O19" s="35">
         <f>SUM(O8:O18)</f>
         <v>71.98</v>
       </c>
@@ -1508,7 +1681,7 @@
       <c r="L23" s="21"/>
       <c r="M23" s="33"/>
       <c r="N23" s="23"/>
-      <c r="O23" s="36"/>
+      <c r="O23" s="35"/>
       <c r="P23" s="33"/>
       <c r="Q23" s="23"/>
     </row>
@@ -1770,12 +1943,12 @@
         <v>35</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="2:15">
       <c r="B2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
         <v>40</v>
@@ -1798,12 +1971,12 @@
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="27" t="s">
         <v>33</v>
       </c>
@@ -1815,13 +1988,13 @@
       </c>
       <c r="K6" s="29"/>
       <c r="L6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="27" t="s">
         <v>46</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>47</v>
       </c>
       <c r="O6" s="27" t="s">
         <v>33</v>
@@ -1848,7 +2021,7 @@
       <c r="K7" s="29"/>
       <c r="L7" s="25"/>
       <c r="M7" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
@@ -2552,161 +2725,478 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="115.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="37"/>
-    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="63"/>
+    <col min="3" max="3" width="9.140625" style="36"/>
+    <col min="4" max="4" width="9.140625" style="49"/>
+    <col min="5" max="5" width="9.140625" style="58"/>
+    <col min="7" max="7" width="12.140625" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="61"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="65"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="62">
+        <v>3</v>
+      </c>
+      <c r="C4" s="39">
+        <v>6.68</v>
+      </c>
+      <c r="D4" s="47">
+        <v>-0.19</v>
+      </c>
+      <c r="E4" s="56">
+        <f>+C4/B4</f>
+        <v>2.2266666666666666</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="66">
+        <v>120878</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="62">
+        <v>4</v>
+      </c>
+      <c r="C5" s="39">
+        <v>11.53</v>
+      </c>
+      <c r="D5" s="47">
+        <v>-0.11</v>
+      </c>
+      <c r="E5" s="56">
+        <f t="shared" ref="E5:E9" si="0">+C5/B5</f>
+        <v>2.8824999999999998</v>
+      </c>
+      <c r="F5" s="40"/>
+      <c r="G5" s="66">
+        <v>265785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="62">
+        <v>5</v>
+      </c>
+      <c r="C6" s="39">
+        <v>14.58</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="56">
+        <f t="shared" si="0"/>
+        <v>2.9159999999999999</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="66">
+        <v>281254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="62">
+        <v>3</v>
+      </c>
+      <c r="C7" s="39">
+        <v>7.7</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="56">
+        <f t="shared" si="0"/>
+        <v>2.5666666666666669</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="66">
+        <v>284409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="62">
+        <v>3</v>
+      </c>
+      <c r="C8" s="39">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="56">
+        <f t="shared" si="0"/>
+        <v>5.6633333333333331</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="66">
+        <v>233014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="62">
+        <v>7</v>
+      </c>
+      <c r="C9" s="39">
+        <v>11.69</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="64">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="67">
+        <v>245875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="38"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="68"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="38"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="68"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="65"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="63">
+        <v>10</v>
+      </c>
+      <c r="C13" s="30">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="56">
+        <f t="shared" ref="E13:E15" si="1">+C13/B13</f>
+        <v>1.6989999999999998</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="69">
+        <v>209398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="63">
+        <v>10</v>
+      </c>
+      <c r="C14" s="30">
+        <v>24.34</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="56">
+        <f t="shared" si="1"/>
+        <v>2.4340000000000002</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="70">
+        <v>264070</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="63">
+        <v>10</v>
+      </c>
+      <c r="C15" s="30">
+        <v>15.53</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="64">
+        <f t="shared" si="1"/>
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="67">
+        <v>286736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="20"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="70"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="20"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="48"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="70"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="48"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="70"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="63">
+        <v>12</v>
+      </c>
+      <c r="C19" s="30">
+        <v>14.3</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="56">
+        <f t="shared" ref="E19:E20" si="2">+C19/B19</f>
+        <v>1.1916666666666667</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="70">
+        <v>263808</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="63">
+        <v>12</v>
+      </c>
+      <c r="C20" s="30">
+        <v>11.69</v>
+      </c>
+      <c r="D20" s="48">
+        <v>-0.1</v>
+      </c>
+      <c r="E20" s="56">
+        <f t="shared" si="2"/>
+        <v>0.97416666666666663</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="70">
+        <v>254040</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="20"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="48"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="69"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="48"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="69"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="63">
         <v>60</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="C23" s="30">
+        <v>42.96</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="56">
+        <f t="shared" ref="E23:E25" si="3">+C23/B23</f>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="70">
+        <v>265552</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="63">
+        <v>72</v>
+      </c>
+      <c r="C24" s="30">
+        <v>35.99</v>
+      </c>
+      <c r="D24" s="48"/>
+      <c r="E24" s="56">
+        <f t="shared" si="3"/>
+        <v>0.49986111111111114</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="69">
+        <v>184665</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="19" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="25"/>
-      <c r="B2" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="30">
-        <v>14.3</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="30">
-        <v>11.99</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="30">
-        <v>42.96</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="30">
-        <v>35.99</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="37">
-        <v>21.5</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="20"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="30">
-        <v>24.34</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="30">
+      <c r="B25" s="63">
+        <v>72</v>
+      </c>
+      <c r="C25" s="36">
+        <v>23.16</v>
+      </c>
+      <c r="E25" s="64">
+        <f t="shared" si="3"/>
+        <v>0.32166666666666666</v>
+      </c>
+      <c r="G25" s="67">
+        <v>228618</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="20"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="48"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="69"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="63">
+        <v>60</v>
+      </c>
+      <c r="C28" s="30">
         <v>16.420000000000002</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="E11" s="19" t="s">
-        <v>69</v>
+      <c r="E28" s="56">
+        <f t="shared" ref="E28" si="4">+C28/B28</f>
+        <v>0.27366666666666667</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="70">
+        <v>264422</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-    <hyperlink ref="A3" r:id="rId6"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="A5" r:id="rId8"/>
-    <hyperlink ref="A6" r:id="rId9"/>
-    <hyperlink ref="A9" r:id="rId10"/>
-    <hyperlink ref="E7" r:id="rId11"/>
-    <hyperlink ref="A7" r:id="rId12"/>
-    <hyperlink ref="E11" r:id="rId13"/>
-    <hyperlink ref="A11" r:id="rId14"/>
+    <hyperlink ref="A19" r:id="rId1"/>
+    <hyperlink ref="A20" r:id="rId2"/>
+    <hyperlink ref="A23" r:id="rId3"/>
+    <hyperlink ref="A24" r:id="rId4"/>
+    <hyperlink ref="A14" r:id="rId5"/>
+    <hyperlink ref="A25" r:id="rId6"/>
+    <hyperlink ref="A28" r:id="rId7"/>
+    <hyperlink ref="A13" r:id="rId8" location=".UvEZXlKA2KQ"/>
+    <hyperlink ref="A4" r:id="rId9" location=".UvEZhVKA2KR"/>
+    <hyperlink ref="A5" r:id="rId10" location=".UvEY9FKA2KQ"/>
+    <hyperlink ref="A6" r:id="rId11" location=".UvEZD1KA2KQ"/>
+    <hyperlink ref="A7" r:id="rId12" location=".UvEZHlKA2KQ"/>
+    <hyperlink ref="A8" r:id="rId13" location=".UvEZRFKA2KQ"/>
+    <hyperlink ref="A15" r:id="rId14" location=".UvEl6lKA2KQ"/>
+    <hyperlink ref="A9" r:id="rId15" location=".UvEnIVKA2KQ"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>